<commit_message>
Always cite newest BT
</commit_message>
<xml_diff>
--- a/src/sources.xlsx
+++ b/src/sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\Desktop\IQB\BT-ShinyApp\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8644E68-F631-4B5B-AED9-B3179799B8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{428ED400-F737-4238-9A50-1F889166A7A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>year</t>
   </si>
@@ -33,19 +33,7 @@
     <t>source</t>
   </si>
   <si>
-    <t>Stanat, P., Pant, H. A., Böhme, K., &amp; Richter, D. (Eds.). (2012). *Kompetenzen von Schülerinnen und Schülern am Ende der vierten Jahrgangsstufe in den Fächern Deutsch und Mathematik.* Waxmann. https://www.iqb.hu-berlin.de/bt/LV2011/Bericht/LV_2011_Bericht.pdf</t>
-  </si>
-  <si>
     <t>Köller, O., Knigge, M., &amp; Tesch, B. (2010). *Sprachliche Kompetenzen im Ländervergleich.* Waxmann. http://www.iqb.hu-berlin.de/bt/LV08_09/LV_ZF_0809c.pdf</t>
-  </si>
-  <si>
-    <t>Pant, H. A., Stanat, P., Schroeders, U., Roppelt, A., Siegle, T., &amp; Pöhlmann, C. (Eds.). (2013). *IQB-Ländervergleich 2012. Mathematische und naturwissenschaftliche Kompetenzen am Ende der Sekundarstufe I.* Waxmann. https://www.iqb.hu-berlin.de/bt/lv2012/Bericht/Bericht.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stanat, P., Böhme, K., Schipolowski &amp; Haag, N. (Hrsg.). (2016). *IQB-Bildungstrend 2015: Sprachliche Kompetenzen am Ende der 9. Jahrgangsstufe im zweiten Ländervergleich.* Waxmann Verlag. https://elibrary.utb.de/doi/book/10.31244/9783830985358 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stanat, P., Schipolowski, S., Rjosk, C., Weirich, S. &amp; Haag, N. (Hrsg.). (2017). *IQB-Bildungstrend 2016: Kompetenzen in den Fächern Deutsch und Mathematik am Ende der 4. Jahrgangsstufe im zweiten Ländervergleich.* Waxmann Verlag. https://elibrary.utb.de/doi/book/10.31244/9783830987307 </t>
   </si>
   <si>
     <t xml:space="preserve">Stanat, P., Schipolowski, S., Mahler, N., Weirich, S. &amp; Henschel, S. (2019). *IQB-Bildungstrend 2018. Mathematische und naturwissenschaftliche Kompetenzen am Ende der Sekundarstufe I im zweiten Ländervergleich.* Waxmann Verlag. https://directory.doabooks.org/handle/20.500.12854/50672 </t>
@@ -374,8 +362,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -396,7 +384,7 @@
         <v>2009</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
@@ -404,7 +392,7 @@
         <v>2011</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
@@ -412,7 +400,7 @@
         <v>2012</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -428,7 +416,7 @@
         <v>2016</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
@@ -436,7 +424,7 @@
         <v>2018</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
@@ -444,7 +432,7 @@
         <v>2021</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
@@ -452,7 +440,7 @@
         <v>2022</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 2008 in sources
</commit_message>
<xml_diff>
--- a/src/sources.xlsx
+++ b/src/sources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alina\Desktop\IQB\BT-ShinyApp\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDCBF65-9072-44EA-B93B-544F54ABD888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2FBF1F-42EB-4C07-9FBE-38DB6B872E60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="5">
   <si>
     <t>year</t>
   </si>
@@ -357,10 +357,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -378,7 +378,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2">
-        <v>2009</v>
+        <v>2008</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -386,57 +386,65 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5">
-        <v>2015</v>
+        <v>2012</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A7">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="B7" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A8">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="B8" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A9">
+        <v>2021</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10">
         <v>2022</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>